<commit_message>
Add Homepage to jump into other three pages
</commit_message>
<xml_diff>
--- a/orderrecord.xlsx
+++ b/orderrecord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ccd51aaea1fe508/Documents/Java Projects/02-duckdeng/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{8BC439E1-5175-44EF-94F0-CA43F9B1EB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1B48DD5-EE33-4846-9C0F-4213029C1722}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{8BC439E1-5175-44EF-94F0-CA43F9B1EB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F035C39-0599-4E9A-8CED-796E17710B54}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orderIdwithAmount" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,43 +44,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>全家二吃辣</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>半鴨二吃辣</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全鴨剁炒辣</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>半鴨剁炒辣</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>全鴨剁盤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>半鴨剁盤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全雞手扒雞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>半雞手扒雞</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>荷葉餅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>甜麵醬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -579,38 +543,38 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>280</v>
@@ -626,30 +590,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893FDE67-CD3C-49CB-84A7-61E7EAA1DF3A}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>600</v>
@@ -658,20 +622,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>650</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>320</v>
@@ -680,20 +644,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>350</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>590</v>
@@ -702,20 +666,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>630</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>300</v>
@@ -724,81 +688,81 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>320</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>570</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>290</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>450</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>230</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -812,161 +776,161 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.75" customWidth="1"/>
-    <col min="13" max="13" width="13.75" customWidth="1"/>
-    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>

</xml_diff>